<commit_message>
changes to the templates
</commit_message>
<xml_diff>
--- a/app/www/Camera_data_MDB_share.xlsx
+++ b/app/www/Camera_data_MDB_share.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Ecosystems\Conservation Science\Species Conservation Science\Mesocarnivores\Projects\Mesocarnivore_Monitoring_Program\2.Data\Mesocarnivores DB\3. Database Templates\For Scientists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalR\mdm_form_submission\app\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C38D35C-8288-47F5-A012-C2FDC746876B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B78C16F-4B90-4D1A-988A-DED6B7BC5628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="12624" xr2:uid="{9787400D-7BDC-4090-BF3A-2F27E03ECF78}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="107">
   <si>
     <t>yes</t>
   </si>
@@ -157,9 +157,6 @@
     <t>Study_area</t>
   </si>
   <si>
-    <t>Project_id</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -380,6 +377,9 @@
   </si>
   <si>
     <t>Unique name for the project. E.g., Enterprise Fisher Survey. If you completed the online form, please use the text you used for project name.</t>
+  </si>
+  <si>
+    <t>Enterprise fisher survey</t>
   </si>
 </sst>
 </file>
@@ -627,6 +627,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -660,7 +661,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -993,7 +993,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1016,17 +1016,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
-        <v>105</v>
+      <c r="A1" s="29" t="s">
+        <v>104</v>
       </c>
       <c r="B1" s="22" t="s">
         <v>17</v>
       </c>
       <c r="C1" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>76</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>77</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>16</v>
@@ -1038,7 +1038,7 @@
         <v>13</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I1" s="25" t="s">
         <v>11</v>
@@ -1053,7 +1053,7 @@
         <v>8</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N1" s="9" t="s">
         <v>5</v>
@@ -1063,8 +1063,11 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>106</v>
+      </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2">
         <v>51.576687999999997</v>
@@ -1073,16 +1076,16 @@
         <v>-122.745352</v>
       </c>
       <c r="E2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" t="s">
         <v>93</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" t="s">
         <v>94</v>
-      </c>
-      <c r="G2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H2" t="s">
-        <v>95</v>
       </c>
       <c r="I2" s="26">
         <v>39619</v>
@@ -1097,19 +1100,19 @@
         <v>39460</v>
       </c>
       <c r="M2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N2" t="s">
         <v>98</v>
       </c>
-      <c r="N2" t="s">
-        <v>99</v>
-      </c>
       <c r="O2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B7" s="23"/>
       <c r="C7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1135,21 +1138,21 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1158,13 +1161,13 @@
         <v>42580.264386574076</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="23"/>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1200,33 +1203,33 @@
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>32</v>
+        <v>104</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
@@ -1270,14 +1273,14 @@
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="29" t="s">
-        <v>82</v>
+      <c r="C5" s="30" t="s">
+        <v>81</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>26</v>
@@ -1293,9 +1296,9 @@
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="35"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="30"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="31"/>
       <c r="D6" s="10" t="s">
         <v>23</v>
       </c>
@@ -1310,9 +1313,9 @@
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="36"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="33"/>
+      <c r="A7" s="37"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="10" t="s">
         <v>20</v>
       </c>
@@ -1334,7 +1337,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
@@ -1345,13 +1348,13 @@
     </row>
     <row r="9" spans="1:10" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
@@ -1362,13 +1365,13 @@
     </row>
     <row r="10" spans="1:10" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -1378,20 +1381,20 @@
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:10" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="29" t="s">
-        <v>83</v>
+      <c r="C11" s="30" t="s">
+        <v>82</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="3"/>
@@ -1399,14 +1402,14 @@
       <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:10" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="32"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
       <c r="D12" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="3"/>
@@ -1414,14 +1417,14 @@
       <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="32"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
       <c r="D13" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="3"/>
@@ -1429,14 +1432,14 @@
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="32"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
       <c r="D14" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="3"/>
@@ -1444,14 +1447,14 @@
       <c r="J14" s="3"/>
     </row>
     <row r="15" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="32"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
       <c r="D15" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="3"/>
@@ -1459,14 +1462,14 @@
       <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="32"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
       <c r="D16" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="3"/>
@@ -1474,14 +1477,14 @@
       <c r="J16" s="3"/>
     </row>
     <row r="17" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="32"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
       <c r="D17" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="3"/>
@@ -1489,14 +1492,14 @@
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:10" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="32"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
       <c r="D18" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="3"/>
@@ -1504,14 +1507,14 @@
       <c r="J18" s="3"/>
     </row>
     <row r="19" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="32"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
       <c r="D19" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="3"/>
@@ -1519,14 +1522,14 @@
       <c r="J19" s="3"/>
     </row>
     <row r="20" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="32"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
       <c r="D20" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="3"/>
@@ -1534,14 +1537,14 @@
       <c r="J20" s="3"/>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="32"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
+      <c r="A21" s="33"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
       <c r="D21" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="3"/>
@@ -1549,14 +1552,14 @@
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="32"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
+      <c r="A22" s="33"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
       <c r="D22" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="3"/>
@@ -1564,14 +1567,14 @@
       <c r="J22" s="3"/>
     </row>
     <row r="23" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="32"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
+      <c r="A23" s="33"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
       <c r="D23" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="3"/>
@@ -1579,14 +1582,14 @@
       <c r="J23" s="3"/>
     </row>
     <row r="24" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="32"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
       <c r="D24" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="3"/>
@@ -1594,14 +1597,14 @@
       <c r="J24" s="3"/>
     </row>
     <row r="25" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="32"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="33"/>
+      <c r="A25" s="33"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="34"/>
       <c r="D25" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="3"/>
@@ -1633,7 +1636,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
@@ -1650,7 +1653,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
@@ -1667,7 +1670,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
@@ -1684,7 +1687,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
@@ -1701,7 +1704,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
@@ -1718,7 +1721,7 @@
         <v>0</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
@@ -1780,21 +1783,21 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
@@ -1802,13 +1805,13 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D40" s="19"/>
       <c r="G40" s="3"/>
@@ -1817,13 +1820,13 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D41" s="19"/>
       <c r="G41" s="3"/>
@@ -1832,13 +1835,13 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D42" s="20"/>
       <c r="G42" s="3"/>
@@ -1847,13 +1850,13 @@
     </row>
     <row r="43" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D43" s="20"/>
       <c r="G43" s="3"/>

</xml_diff>